<commit_message>
add all Entity to Lavka
</commit_message>
<xml_diff>
--- a/Table.xlsx
+++ b/Table.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/Toleran/Proect_Lavka/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72E61F3-5421-BF4D-A2B7-7CD4FEA01C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B830AF-3317-F641-A051-1B3926B9D65C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{B0C12B5B-BDC3-3D44-9FC6-91DA3CA8AE20}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17160" xr2:uid="{B0C12B5B-BDC3-3D44-9FC6-91DA3CA8AE20}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="201">
   <si>
     <r>
       <t xml:space="preserve">name </t>
@@ -624,9 +624,6 @@
     <t xml:space="preserve">номер склада на котором проведен документ </t>
   </si>
   <si>
-    <t>id_TT bigint</t>
-  </si>
-  <si>
     <t xml:space="preserve">дальше таблицы связанные с прогнозом - они уже не связаны с шаблонами </t>
   </si>
   <si>
@@ -739,13 +736,76 @@
   </si>
   <si>
     <t>если прогноз больше чем реальные продажи , то во сколько раз больше можно заказать чем цыфра реальных продаж</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> int</t>
+  </si>
+  <si>
+    <t>прогноз на количество дней</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name_TT </t>
+  </si>
+  <si>
+    <t>varchar(40)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id Склада номер склада - сквозной для всей программы, берем из источника </t>
+  </si>
+  <si>
+    <t>включать или исключать данный вид документа из статистики влияющей на заказ возможен либо у всех true либо у всех false. При true - выбираем документы равные этому условию , при false все документы кроме этих</t>
+  </si>
+  <si>
+    <t>начало анализа</t>
+  </si>
+  <si>
+    <t>конец анализа</t>
+  </si>
+  <si>
+    <t>заказ на это кол-во дней</t>
+  </si>
+  <si>
+    <t xml:space="preserve">supplier </t>
+  </si>
+  <si>
+    <t>varchar(50)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">заказ ограничивается максимумом - реальные продажи * на этот коэфициент </t>
+  </si>
+  <si>
+    <t>Мы перед заказом выбираем какой шаблон использовать и на какого поставщика</t>
+  </si>
+  <si>
+    <t>название склада</t>
+  </si>
+  <si>
+    <t>роль склада (РТ , Приемка..)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name_stock </t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>name_TT</t>
+  </si>
+  <si>
+    <t>stock_tip_sale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOP2_ARTIC </t>
+  </si>
+  <si>
+    <t>поставщик</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -797,6 +857,12 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6AAB73"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -836,37 +902,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1201,1050 +1265,1115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2991E274-B22D-364F-BB9D-7FFB435506CC}">
-  <dimension ref="A1:D122"/>
+  <dimension ref="A1:D125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="223" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="223" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="40.6640625" style="4" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:4" s="11" customFormat="1">
+      <c r="A5" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="51">
+      <c r="A10" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="B9" s="4" t="s">
+    </row>
+    <row r="13" spans="1:4" s="11" customFormat="1">
+      <c r="A13" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="85">
+      <c r="A16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17">
+      <c r="A17" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B17" t="s">
+        <v>183</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="34">
+      <c r="A18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="17">
+      <c r="A19" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17">
+      <c r="A20" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B20" t="s">
+        <v>132</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="17">
+      <c r="A21" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" t="s">
+        <v>134</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="17">
+      <c r="A22" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22" t="s">
+        <v>134</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="17">
+      <c r="A23" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B23" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="3"/>
+      <c r="C24" s="4"/>
+    </row>
+    <row r="26" spans="1:3" s="11" customFormat="1" ht="51">
+      <c r="A26" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="51">
+      <c r="A29" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B29" t="s">
+        <v>116</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="85">
+      <c r="A31" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="3"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="15" customFormat="1" ht="68">
+      <c r="A35" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>86</v>
+      </c>
+      <c r="B39" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
+      <c r="C39" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="34">
+      <c r="A42" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="34">
+      <c r="A43" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B43" t="s">
+        <v>190</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="85">
+      <c r="A45" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="4" t="s">
+      <c r="B45" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B14" s="4" t="s">
+    <row r="47" spans="1:3">
+      <c r="A47" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B47" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="85" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="C47" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B48" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="C48" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="B49" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="17">
+      <c r="A50" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B50" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C50" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="C17" s="5" t="s">
+    <row r="51" spans="1:3" ht="34">
+      <c r="C51" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+    <row r="52" spans="1:3" ht="17">
+      <c r="A52" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B52" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C52" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+    <row r="53" spans="1:3" ht="17">
+      <c r="A53" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B53" t="s">
         <v>132</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C53" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+    <row r="54" spans="1:3" ht="17">
+      <c r="A54" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B54" t="s">
         <v>134</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C54" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+    <row r="55" spans="1:3" ht="17">
+      <c r="A55" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B55" t="s">
         <v>134</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C55" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+    <row r="56" spans="1:3" ht="17">
+      <c r="A56" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B56" t="s">
         <v>134</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C56" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="5"/>
-    </row>
-    <row r="25" spans="1:3" s="13" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A25" s="18" t="s">
+    <row r="57" spans="1:3">
+      <c r="A57" s="3"/>
+    </row>
+    <row r="59" spans="1:3" s="11" customFormat="1" ht="68">
+      <c r="A59" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="B59" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B60" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+    <row r="61" spans="1:3">
+      <c r="A61" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B61" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
+      <c r="C61" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="51">
+      <c r="A62" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B62" t="s">
         <v>116</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C62" s="4" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+    <row r="63" spans="1:3">
+      <c r="A63" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B63" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C63" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
+    <row r="64" spans="1:3" ht="34">
+      <c r="A64" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B64" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C64" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="3"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
+    <row r="65" spans="1:3">
+      <c r="A65" s="3"/>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B68" t="s">
+        <v>3</v>
+      </c>
+      <c r="C68" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B69" t="s">
+        <v>22</v>
+      </c>
+      <c r="C69" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B70" t="s">
+        <v>24</v>
+      </c>
+      <c r="C70" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B71" t="s">
+        <v>26</v>
+      </c>
+      <c r="C71" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B72" t="s">
+        <v>26</v>
+      </c>
+      <c r="C72" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B73" t="s">
+        <v>29</v>
+      </c>
+      <c r="C73" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="68">
+      <c r="A74" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B74" t="s">
+        <v>26</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="102">
+      <c r="A75" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B75" t="s">
+        <v>26</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="51">
+      <c r="A76" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B76" t="s">
+        <v>26</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="17">
+      <c r="A77" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B77" t="s">
+        <v>190</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="34">
+      <c r="A78" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B78" t="s">
+        <v>34</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="119">
+      <c r="A79" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B79" t="s">
+        <v>36</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="17">
+      <c r="A80" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B80" t="s">
+        <v>36</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="34">
+      <c r="A81" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B81" t="s">
+        <v>36</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="17">
+      <c r="A83" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="17">
+      <c r="A84" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B84" t="s">
+        <v>54</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B85" t="s">
+        <v>56</v>
+      </c>
+      <c r="C85" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="51">
+      <c r="A86" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B86" t="s">
+        <v>8</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B87" t="s">
+        <v>8</v>
+      </c>
+      <c r="C87" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="34">
+      <c r="A88" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B88" t="s">
+        <v>8</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B89" t="s">
+        <v>8</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B90" t="s">
+        <v>8</v>
+      </c>
+      <c r="C90" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B91" t="s">
+        <v>8</v>
+      </c>
+      <c r="C91" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" s="13" customFormat="1">
+      <c r="A92" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="34">
+      <c r="A95" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B95" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C95" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="17">
+      <c r="A96" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B96" t="s">
+        <v>54</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="17">
+      <c r="A97" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B97" t="s">
+        <v>8</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="17">
+      <c r="A98" s="3" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" s="19" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A34" s="6" t="s">
+      <c r="B98" t="s">
+        <v>145</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="17">
+      <c r="A99" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B99" t="s">
+        <v>56</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="17">
+      <c r="A100" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B100" t="s">
+        <v>8</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="17">
+      <c r="A101" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B101" t="s">
+        <v>61</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="17">
+      <c r="A102" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B102" t="s">
+        <v>26</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="68">
+      <c r="A103" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B103" t="s">
+        <v>148</v>
+      </c>
+      <c r="C103" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="17">
+      <c r="A104" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B104" t="s">
+        <v>7</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" s="11" customFormat="1" ht="34">
+      <c r="A107" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="3"/>
-    </row>
-    <row r="44" spans="1:3" ht="85" x14ac:dyDescent="0.2">
-      <c r="A44" s="18" t="s">
+      <c r="B107" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C107" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="17">
+      <c r="A108" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B108" t="s">
+        <v>14</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="17">
+      <c r="A109" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B109" t="s">
+        <v>159</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="51">
+      <c r="A110" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B110" t="s">
+        <v>26</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="17">
+      <c r="A111" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B111" t="s">
+        <v>26</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" s="12"/>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" s="12"/>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" s="11" customFormat="1">
+      <c r="A121" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B44" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="C49" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="3"/>
-    </row>
-    <row r="57" spans="1:3" s="13" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A57" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B57" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="C57" s="11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A60" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A62" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="3"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B65" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A72" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="102" x14ac:dyDescent="0.2">
-      <c r="A73" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A74" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A75" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="119" x14ac:dyDescent="0.2">
-      <c r="A76" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A77" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A78" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A80" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C80" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A81" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A83" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A85" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C85" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C86" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C87" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C88" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="14" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A92" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B92" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C92" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A93" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C93" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A94" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C94" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A95" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B95" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C95" s="5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A96" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B96" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C96" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A97" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B97" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C97" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A98" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B98" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C98" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A99" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B99" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C99" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A100" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B100" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C100" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A101" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B101" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C101" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A104" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B104" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="C104" s="11" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A105" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B105" s="4" t="s">
+      <c r="B121" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="C121" s="11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B122" t="s">
         <v>14</v>
       </c>
-      <c r="C105" s="5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A106" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B106" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="C106" s="5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A107" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="B107" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C107" s="5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A108" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B108" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C108" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A109" s="14" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A110" s="14"/>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A111" s="14"/>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A112" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A113" s="3" t="s">
+      <c r="C122" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B123" t="s">
+        <v>14</v>
+      </c>
+      <c r="C123" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B124" t="s">
+        <v>166</v>
+      </c>
+      <c r="C124" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" s="13" customFormat="1">
+      <c r="A125" s="12" t="s">
         <v>177</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A114" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A115" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A116" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A117" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B118" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="C118" s="13" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A119" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="B119" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C119" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A120" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="B120" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C120" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A121" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="B121" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="C121" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="14" t="s">
-        <v>178</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2256,96 +2385,96 @@
       <selection activeCell="A9" sqref="A9:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="10"/>
-    </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>85</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1">
       <c r="A17" s="2" t="s">
         <v>11</v>
       </c>
@@ -2363,40 +2492,40 @@
       <selection activeCell="A30" sqref="A1:XFD30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="22.33203125" customWidth="1"/>
     <col min="3" max="3" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:4" s="11" customFormat="1">
+      <c r="A5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -2404,7 +2533,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>99</v>
       </c>
@@ -2415,7 +2544,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -2426,23 +2555,23 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
+    <row r="12" spans="1:4" s="11" customFormat="1">
+      <c r="A12" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="11" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -2450,7 +2579,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
         <v>103</v>
       </c>
@@ -2461,80 +2590,80 @@
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="85">
       <c r="A15" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="34">
       <c r="A16" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="17">
       <c r="A17" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="17">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="17">
       <c r="A19" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="17">
       <c r="A20" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="17">
       <c r="A21" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="17"/>
-    </row>
-    <row r="24" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="C22" s="4"/>
+    </row>
+    <row r="24" spans="1:3" ht="51">
       <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B24" t="s">
         <v>112</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
@@ -2542,7 +2671,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26" s="2" t="s">
         <v>114</v>
       </c>
@@ -2553,18 +2682,18 @@
         <v>119</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="51">
       <c r="A27" s="2" t="s">
         <v>115</v>
       </c>
       <c r="B27" t="s">
         <v>116</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="4" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3">
       <c r="A28" s="2" t="s">
         <v>117</v>
       </c>
@@ -2575,18 +2704,18 @@
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="51">
       <c r="A29" s="2" t="s">
         <v>118</v>
       </c>
       <c r="B29" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3">
       <c r="A30" s="2" t="s">
         <v>11</v>
       </c>

</xml_diff>